<commit_message>
apex reworked for 4 TCDS links
</commit_message>
<xml_diff>
--- a/examples/apex_USp/src/apex_ku15p_root_gty_gth.xlsx
+++ b/examples/apex_USp/src/apex_ku15p_root_gty_gth.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="apex_ku15p_gty_root_config_2" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="118">
   <si>
     <t xml:space="preserve">// path</t>
   </si>
@@ -187,6 +187,15 @@
   </si>
   <si>
     <t xml:space="preserve">count of devices in the system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mem_base</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">memory base for PCIe systems</t>
   </si>
   <si>
     <t xml:space="preserve">apex_ku15p_gth_root.tab</t>
@@ -484,8 +493,8 @@
   </sheetPr>
   <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -716,6 +725,17 @@
       </c>
       <c r="C21" s="0" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="1048523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -790,8 +810,8 @@
   </sheetPr>
   <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -815,7 +835,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -864,7 +884,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>14</v>
@@ -875,7 +895,7 @@
         <v>15</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>17</v>
@@ -886,7 +906,7 @@
         <v>18</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>20</v>
@@ -897,7 +917,7 @@
         <v>21</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>23</v>
@@ -908,7 +928,7 @@
         <v>24</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>26</v>
@@ -919,7 +939,7 @@
         <v>27</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>29</v>
@@ -930,7 +950,7 @@
         <v>30</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>32</v>
@@ -941,7 +961,7 @@
         <v>33</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>35</v>
@@ -952,7 +972,7 @@
         <v>36</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>38</v>
@@ -963,7 +983,7 @@
         <v>39</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>41</v>
@@ -985,7 +1005,7 @@
         <v>44</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>46</v>
@@ -996,7 +1016,7 @@
         <v>47</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>49</v>
@@ -1022,6 +1042,17 @@
       </c>
       <c r="C21" s="0" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="1048523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1097,7 +1128,7 @@
   <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
+      <selection pane="topLeft" activeCell="C25" activeCellId="1" sqref="A22:C22 C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1109,218 +1140,218 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="3" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="3" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="3" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="1" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="1" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="1" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="1" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>